<commit_message>
Missing Rows : Problem Solved
</commit_message>
<xml_diff>
--- a/script_for_suprim_court_data/courtdata.xlsx
+++ b/script_for_suprim_court_data/courtdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J166"/>
+  <dimension ref="A1:J214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8288,52 +8288,52 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>१४</t>
+          <t>१६</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>०६९-CI-१२६५</t>
+          <t>०६९-WO-१३८०</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>१२१०६५</t>
+          <t>१२०९४९</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>२०७०-०३-२०</t>
+          <t>२०७०-०३-२१</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>रिट निवेदन</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>हक कायम</t>
+          <t>उत्प्रेषण</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>मु।स।गर्ने द्धारिका लाल श्रेष्ठ</t>
+          <t>अधिवक्ता श्रीप्रसाद पण्िडत</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>मु।स। गर्ने बाल हरि रावल र लोकरत्न तुलाधर</t>
+          <t>मन्त्रपिरषिदका अध्यक्ष प्रधानमन्त्रि तथा मन्त्रपिरषिदको कार्यालय समेत ५</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>२०७१-०८-१७</t>
+          <t>२०७१-१०-२१</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121065.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_120949.pdf</t>
         </is>
       </c>
     </row>
@@ -8600,282 +8600,282 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>१५</t>
+          <t>२२</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>०६९-CI-१२८८</t>
+          <t>०६९-CR-१०५७</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>१२१२६३</t>
+          <t>१२१०२०</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>२०७०-०३-२४</t>
+          <t>२०७०-०३-२१</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>निर्णय वदर</t>
+          <t>कर्तव्य ज्यान</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>इन्द्रकुमारी देवी चौधरीको हकमा हरेन्द्र कुमार चौधरी</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>नारायण प्रसाद थारु</t>
+          <t>श्याम बहादुर राना , जंगबहादुर श्रेष्ठ र दलबहादुर भन्ने दिल बहादुर रेश्मी</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>२०७२-१२-२३</t>
+          <t>२०७२-०६-०७</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121263.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121020.pdf</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>१६</t>
+          <t>२३</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>०६९-CI-१२८७</t>
+          <t>०६९-CR-१०५४</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>१२१२५४</t>
+          <t>१२१०१७</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>२०७०-०३-२४</t>
+          <t>२०७०-०३-२१</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>अपुताली हक कायम</t>
+          <t>जवरजस्ती करणी</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>इन्द्र कुमारी देवी चौधरीको हकमा हरेन्द्र कुमार चौधरी</t>
+          <t>सन्तोष ुसुन्दास दर्जी</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>नारायण प्रसाद थारु</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>२०७२-१२-२३</t>
+          <t>२०७२-०८-२०</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121254.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121017.pdf</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>१८</t>
+          <t>२</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>०६९-WO-१३८८</t>
+          <t>०६९-RC-०११९</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>१२१००२</t>
+          <t>१२१११६</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>२०७०-०३-२४</t>
+          <t>२०७०-०३-२३</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>कर्तव्य ज्यान</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>ज्ञान बहादुर बम्जन समेत ४</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>अख्तियार दुरुपयोग अनुसन्धान आयोग समेत ३</t>
+          <t>साम्बा तामाङ</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>२०७३-०४-१७</t>
+          <t>२०७०-११-०९</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121002.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121116.pdf</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>६</t>
+          <t>३</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>०६९-WO-१३९९</t>
+          <t>०६९-CI-१२८०</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>१२१०९९</t>
+          <t>१२११५२</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>२०७०-०३-२५</t>
+          <t>२०७०-०३-२३</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>परमादेश</t>
+          <t>उत्प्रेषण</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>अधिवक्ता देवकी पोखरेल समेत ९</t>
+          <t>राजश्व अनुसन्धान वभिाग हरिहर भवन, पुल्चोक ललितपुरका तर्फबाट ऐ।वभिागका महानिर्देशक खुमराज पुञ्जाली</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>अर्थ मन्त्रालय समेत ३</t>
+          <t>काष्ठमण्डप डेभलपमेन्ट बैंक लिमिटेड काठमाडौं</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>२०७१-०७-३०</t>
+          <t>२०७१-०१-२५</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121099.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121152.pdf</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>१७</t>
+          <t>१४</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>०६९-WO-१३९२</t>
+          <t>०६९-CR-१०६५</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>१२१०५६</t>
+          <t>१२११३७</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>२०७०-०३-२५</t>
+          <t>२०७०-०३-२३</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>करकाप</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>तेजनाथ रिमाल समेत ५</t>
+          <t>गगनदेव यादव</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>जि।वि।स।को कार्यालय पर्वत कुश्मा समेत २</t>
+          <t>बद्री नारायण साह</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>२०७२-०१-१०</t>
+          <t>२०७१-०८-०४</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121056.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121137.pdf</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>२९</t>
+          <t>१५</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>०६९-CI-१२९४</t>
+          <t>०६९-CI-१२७८</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>१२१२८५</t>
+          <t>१२१११३</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>२०७०-०३-२५</t>
+          <t>२०७०-०३-२३</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -8885,49 +8885,49 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>अन्य</t>
+          <t>लेनदेन</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>सुरेन्द्र कुमार लिम्बु</t>
+          <t>गगनदेव यादव र श्याम सुन्दर यादव</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>नरसिंह बहादुर लिम्बु</t>
+          <t>बद्री नारायण शाह</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>२०७३-०९-०६</t>
+          <t>२०७१-०८-०४</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121285.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121113.pdf</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>३३</t>
+          <t>१४</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>०६९-CR-१०७७</t>
+          <t>०६९-CR-१०७५</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>१२१४००</t>
+          <t>१२१२४८</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>२०७०-०३-२५</t>
+          <t>२०७०-०३-२४</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -8937,79 +8937,79 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>जिउ मास्ने बेच्ने</t>
+          <t>जालसाजी</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>र्इन्द्र कुमारी देवी चौधरीको हकमा हरेन्द्र कुमार चौधरी</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>कमल अधिकारी</t>
+          <t>नारायण प्रसाद थारु समेत १२</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>२०७४-०५-२६</t>
+          <t>२०७२-१२-२३</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121400.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121248.pdf</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>१३</t>
+          <t>१५</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>०६९-RC-०१२१</t>
+          <t>०६९-CI-१२८८</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>१२१३२७</t>
+          <t>१२१२६३</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>२०७०-०३-२८</t>
+          <t>२०७०-०३-२४</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>कर्तव्य ज्यान</t>
+          <t>निर्णय वदर</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>इन्द्रकुमारी देवी चौधरीको हकमा हरेन्द्र कुमार चौधरी</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>रामकुमार रार्इ</t>
+          <t>नारायण प्रसाद थारु</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>२०७०-०५-२१</t>
+          <t>२०७२-१२-२३</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121327.pdf</t>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121263.pdf</t>
         </is>
       </c>
     </row>
@@ -9021,47 +9021,2543 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>०६९-WS-००८६</t>
+          <t>०६९-CI-१२८७</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>१२११७७</t>
+          <t>१२१२५४</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>२०७०-०३-२८</t>
+          <t>२०७०-०३-२४</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>अपुताली हक कायम</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>इन्द्र कुमारी देवी चौधरीको हकमा हरेन्द्र कुमार चौधरी</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>नारायण प्रसाद थारु</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>२०७२-१२-२३</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121254.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३८८</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>१२१००२</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
           <t>रिट निवेदन</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr">
+      <c r="F167" t="inlineStr">
         <is>
           <t>उत्प्रेषण</t>
         </is>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>अधिवक्ता जयमंगल प्रसाद</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>सम्माननीय अध्यक्ष, नेपाल सरकार प्रधानमन्त्री तथा मन्त्रीपरिषद कार्यालय समेत १०</t>
-        </is>
-      </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>२०७१-१२-१२</t>
-        </is>
-      </c>
-      <c r="J166" t="inlineStr">
-        <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121177.pdf</t>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>ज्ञान बहादुर बम्जन समेत ४</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>अख्तियार दुरुपयोग अनुसन्धान आयोग समेत ३</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>२०७३-०४-१७</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121002.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२८९</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>१२१२६७</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>कित्ता काट</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>रञ्िजत कोइराला</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>मिश्री खड्का</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>२०७३-११-०३</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121267.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>२०</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०७६</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>१२१३९७</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>भ्रष्टाचार</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>शम्भु भारती</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>२०७४-०१-१७</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121397.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>२१</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२९०</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>१२१२७१</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>निषेधाज्ञा</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>नेपाल दुरसंचार कम्पनी लिमिटेड र ऐ।ऐ।का प्रवन्धक निर्देशकका तर्फबाट अख्तियार प्राप्त अमरनाथ सिंह समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>चक्रलाल श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>२०७४-१०-२८</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121271.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>२२</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२८६</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>१२११७४</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>वकसपत्र</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>माहामती देवी खड्का र महेन्द्र सिंह खड्का</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>मेघराज खड्का</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>२०७५-०३-०८</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121174.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>२३</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९०</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>१२१००७</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२४</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>मोइनुद्दिन बागवान</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>पुनरावेदन अदालत नेपालगंज समेत ५</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>२०७६-०७-०४</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121007.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>३</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९६</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>१२१०९४</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>टेम्पल आर्ट एक्सपोजिशनका अ।प्रा।स। नवराज नेपाल</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>लक्ष्मी बैंक लिमिटेड समेत २</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>२०७०-०९-०९</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121094.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>६</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९९</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>१२१०९९</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>अधिवक्ता देवकी पोखरेल समेत ९</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>अर्थ मन्त्रालय समेत ३</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>२०७१-०७-३०</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121099.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>१७</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९२</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>१२१०५६</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>तेजनाथ रिमाल समेत ५</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>जि।वि।स।को कार्यालय पर्वत कुश्मा समेत २</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121056.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>२९</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२९४</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>१२१२८५</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>अन्य</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>सुरेन्द्र कुमार लिम्बु</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>नरसिंह बहादुर लिम्बु</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>२०७३-०९-०६</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121285.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>३३</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०७७</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>१२१४००</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>जिउ मास्ने बेच्ने</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>कमल अधिकारी</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>२०७४-०५-२६</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121400.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>३४</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>०६९-WS-००८४</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>१२१०९२</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>रामजीवन साह सोनार समेत ११</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>प्रधानमन्त्री तथा मन्त्रीपरिषद कार्यालय समेत ५</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>२०७४-०९-२६</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121092.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>३५</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२९१</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>१२१२७९</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>अन्य</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>मु।स। गर्ने रिद्धि थापा घले</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>गंगाराम खड्गी</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>२०७४-११-०६</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121279.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>३६</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२९२</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>१२१२८०</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>विविध</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>मु।स।गर्ने रिद्धि थापा घले</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>गंगाराम खड्गी</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>२०७४-११-०६</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121280.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>३७</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९८</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>१२१०९८</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>गोपाल रसायली</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>सहरी विकास मन्त्रालय समेत ३</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>२०७४-०९-२६</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121098.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>३८</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>०६९-WO-१३९४</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>१२१०७४</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>विविध</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>अधिवक्ता सुनिल कुमार पटेल समेत २</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>सम्माननीय अन्तरिम चुनावी मन्त्रीपरषदिका अध्यक्ष, प्रधानमन्त्री तथा मन्त्रीपरषदि कार्यालय समेत ४</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>२०७५-०९-०४</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121074.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>३९</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>०६९-RB-००६९</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>१२१२५१</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२५</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>राजस्व र बाणिज्य</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>राजस्व र वाणिज्य</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>राजेन्द्र कुमार थापा</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>मिल बहादुर कायथ्ठ</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>२०७६-०९-१४</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121251.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>३</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>०६९-CI-१२९९</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>१२१३०८</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>मोही लगत कट्टा</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>गोकर्ण प्रसाद जोशी</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>ढोगे नाउं</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>२०७१-०९-२५</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121308.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>४</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>०६९-CI-१३००</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>१२१३१२</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>मोही नामसारी</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>गोकर्ण प्रसाद जोशी</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>भुर्रा नाउं</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>२०७१-०९-२५</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121312.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>१०</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>०६९-WS-००८५</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>१२१११९</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>अधिवक्ता पूर्णचन्द्र पौडेल</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>निर्वाचन आयोग बहादुर भवन समेत</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>२०७२-०५-१०</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121119.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>११</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४०४</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>१२११३५</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>शरणहरि जोशी समेत ४१</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>प्रधानमन्त्रि तथा मन्त्रपिरिषदको कार्यालय समेत १२</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>२०७२-०८-१६</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121135.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>१३</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>०६९-RC-०१२०</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>१२११५४</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>कर्तव्य ज्यान</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>रेसम भन्ने सुवास महरा</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>२०७२-१०-०४</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121154.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>१४</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>०६९-RB-००७०</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>१२१३१६</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२६</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>राजस्व र बाणिज्य</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>राजस्व र वाणिज्य</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>राधाकृष्ण कार्की</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>ऐ।ऐ। को संचालक समिति , जिल्ला विकास समितिको कार्यालय सिन्धुपाल्चोक र ऐ।कार्यालयका स्थानिय विकास अधिकारी</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>२०७३-०५-२३</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121316.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>९</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८०</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>१२१४०६</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>लागु ‌‌औषधी हिरोइन</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>मान बहादुर खड्का</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>२०७१-०३-०९</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121406.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८२</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>१२१४०९</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>नक्कली प्रमाण पत्र</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>रुद्रबहादुर वली</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>२०७२-०६-१९</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121409.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४०६</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>१२११४७</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>मध्यमाञ्चल बोन र्इन्डष्टि्रजका साझेदार राज कुमार शाह समेत २</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>उद्योग मन्त्रालय सिंहदरवार समेत ४</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>२०७२-०९-१३</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121147.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>२४</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०७९</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>१२१४०४</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>भ्रष्टाचार</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>ओम विक्रम राणा</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>२०७४-०१-१७</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121404.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>२५</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८१</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>१२१४०८</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>बैंकिङ्ग कसुर</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>अच्यूत प्रसाद भट्रार्इ</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>२०७५-१२-१३</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121408.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>९</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८०</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>१२१४०६</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>लागु ‌‌औषधी हिरोइन</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>मान बहादुर खड्का</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>२०७१-०३-०९</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121406.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८२</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>१२१४०९</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>नक्कली प्रमाण पत्र</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>रुद्रबहादुर वली</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>२०७२-०६-१९</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121409.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४०६</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>१२११४७</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>मध्यमाञ्चल बोन र्इन्डष्टि्रजका साझेदार राज कुमार शाह समेत २</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>उद्योग मन्त्रालय सिंहदरवार समेत ४</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>२०७२-०९-१३</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121147.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>२४</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०७९</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>१२१४०४</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>भ्रष्टाचार</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>ओम विक्रम राणा</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>२०७४-०१-१७</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121404.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>२५</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०८१</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>१२१४०८</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>२०७०-०३-२७</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>बैंकिङ्ग कसुर</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>अच्यूत प्रसाद भट्रार्इ</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>२०७५-१२-१३</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121408.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>८</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४२८</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>१२१२४३</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>नानीराम हुमागार्इ</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>गृह मन्त्रालय सिंहदरवार समेत ५</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>२०७१-०५-०२</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121243.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>९</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१४</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>१२१४३०</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>लिखत वदर</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>रेशमान तुलाधर समेत ५ जना , मु।स। गर्ने पदमशोभा तुलाधर , मु।स। गर्ने सुमित्रा राजकर्णीकार तुलाधर र सुमन तुलाधर</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>ज्ञानेन्द्ररत्न तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121430.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>१०</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१५</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>१२१४३५</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>दर्ता फारी</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>मैखु गुरुङ र छोमा गुरुङ</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>ज्ञानेन्द्ररत्न तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121435.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>११</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१६</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>१२१४३७</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>दर्ता फारी</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>पूर्णलाल श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>ज्ञानेन्द्ररत्न तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121437.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>१२</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१९</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>१२१४५०</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>लिखत वदर</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>रेशमान तुलाधर समेत ६</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>ज्ञानेन्द्ररत्न तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121450.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>१३</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१८</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>१२१४४२</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>गुठी धर्मलोप</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>रेशमान तुलाधर , मु।स। गर्ने पद्मशोभा तुलाधर , मु।स। गर्ने सुमित्रा राजकणिकार ढतुलाधरण् र सुमन तुलाधर</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>डा।ज्ञानेन्द्ररत्न तुलाधर</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121442.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>१४</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>०६९-NF-००१७</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>१२१४३८</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>लिखत वदर</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>रेशमान तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>ज्ञानेन्द्ररत्न तुलाधर समेत ५ जना</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>२०७२-०१-१०</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121438.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>१५</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४२६</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>१२१२३५</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>रातो कुमारी विकास सेवा समितिका अ।प्रा।स।अशोक तण्डुकार समेत ४</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>प्रधानमन्त्रि तथा मन्त्रपिरिषदको कार्यालय समेत १०</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>२०७३-०६-०५</t>
+        </is>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121235.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>१६</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>०६९-CR-१०९१</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>१२१४१८</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>अदालतको अवहेलना</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>नेम इन्स्टीच्युट फर मेडिकल एजुकेशन प्रा।लि।को तर्फबाट अख्तियार प्राप्त संचालक डा।नविन कुमार शर्मा</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>मनोज कुमार सिंह</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>२०७३-१२-२१</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121418.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>१७</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४२९</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>१२१२४७</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>जागेश्वर शाह</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>लोक सेवा आयोग केन्द्रिय कार्यालय समेत ४</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>२०७४-०२-०१</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121247.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४२७</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>१२१२३९</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>उमा पौडेल समेत ५</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>मन्त्रपिरषिद प्रधानमन्त्र ितथा मन्त्रपिरषिदको कार्यालय समेत ६</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>२०७४-०९-२१</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121239.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>२२</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>०६९-CI-१३०५</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>१२१३३८</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३०</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>अन्य</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>रमादेवी ढकाल र आफनो हकमा समेत अच्युतम प्रसाद उपाध्याय ढकाल</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>जानकीदेवी ढकाल , विष्णु कुमार ढकाल र हरिहर कुमार ढकाल</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>२०७६-११-१९</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121338.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>२८</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>०६९-CI-१३०८</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>१२१४५८</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३१</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>लेनदेन</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>टिका बहादुर वली</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>धनिराम खड्का</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>२०७०-११-२०</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121458.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>३२</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४३४</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>१२१३३७</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३१</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>लक्ष्मी इन्टरकन्टिनेन्टल प्रा।ली</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>भौतिक पूर्वाधार तथा यातायात व्यवस्था मन्त्रालय सिंहदरवार समेत</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>२०७१-१०-११</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121337.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>३७</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>०६९-WO-१४३३</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>१२१३२९</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>२०७०-०३-३१</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>हरि बहादुर रोकाया</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>प्रधानमन्त्रि तथा मन्त्रपिरिषदको कार्यालय समेत ८</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>२०७४-१२-०६</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_121329.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>